<commit_message>
icc analysis added to pipeline
</commit_message>
<xml_diff>
--- a/data/TROOPS-ratings.xlsx
+++ b/data/TROOPS-ratings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21421"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10504"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T57361~1\AppData\Local\Temp\7zO4391EAE7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaronconway/TROOPS-reliability/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="518" documentId="11_F5DA53B5A18D182C9524FE569FB58A3F247C0BFB" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{648F2308-217F-4ADB-974E-8AFD4CECFBF3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8550334F-1227-244E-8296-0A363505E69F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
@@ -148,7 +148,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -478,26 +478,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J402"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A290" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A329" sqref="A329:XFD329"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="8.85546875" style="1"/>
-    <col min="3" max="3" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="8.83203125" style="1"/>
+    <col min="3" max="3" width="15.5" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" style="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5" style="1" customWidth="1"/>
     <col min="8" max="8" width="12" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="1"/>
+    <col min="9" max="9" width="10.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10.1640625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30">
+    <row r="1" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -529,7 +529,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="69.75" customHeight="1">
+    <row r="2" spans="1:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -558,7 +558,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -572,7 +572,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -586,7 +586,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -600,7 +600,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -611,7 +611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="60">
+    <row r="7" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -640,7 +640,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -654,7 +654,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -668,7 +668,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -682,7 +682,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -693,7 +693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>2</v>
       </c>
@@ -707,7 +707,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>2</v>
       </c>
@@ -721,7 +721,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>2</v>
       </c>
@@ -735,7 +735,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>2</v>
       </c>
@@ -749,7 +749,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>2</v>
       </c>
@@ -760,7 +760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>2</v>
       </c>
@@ -774,7 +774,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>2</v>
       </c>
@@ -788,7 +788,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>2</v>
       </c>
@@ -802,7 +802,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>2</v>
       </c>
@@ -816,7 +816,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>2</v>
       </c>
@@ -827,7 +827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>3</v>
       </c>
@@ -841,7 +841,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>3</v>
       </c>
@@ -855,7 +855,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>3</v>
       </c>
@@ -869,7 +869,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>3</v>
       </c>
@@ -883,7 +883,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>3</v>
       </c>
@@ -891,7 +891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="36" customHeight="1">
+    <row r="27" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>3</v>
       </c>
@@ -908,7 +908,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>3</v>
       </c>
@@ -922,7 +922,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>3</v>
       </c>
@@ -936,7 +936,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>3</v>
       </c>
@@ -950,7 +950,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>3</v>
       </c>
@@ -961,7 +961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>4</v>
       </c>
@@ -975,7 +975,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>4</v>
       </c>
@@ -989,7 +989,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>4</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>4</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>4</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>4</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>4</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>4</v>
       </c>
@@ -1070,7 +1070,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>4</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>4</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="34.5" customHeight="1">
+    <row r="42" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>5</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>5</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>5</v>
       </c>
@@ -1140,7 +1140,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>5</v>
       </c>
@@ -1154,7 +1154,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>5</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>5</v>
       </c>
@@ -1179,7 +1179,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>5</v>
       </c>
@@ -1193,7 +1193,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>5</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>5</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>5</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>6</v>
       </c>
@@ -1246,7 +1246,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>6</v>
       </c>
@@ -1260,7 +1260,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>6</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>6</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>6</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>6</v>
       </c>
@@ -1310,7 +1310,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>6</v>
       </c>
@@ -1324,7 +1324,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>6</v>
       </c>
@@ -1338,7 +1338,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>6</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>6</v>
       </c>
@@ -1360,7 +1360,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>7</v>
       </c>
@@ -1374,7 +1374,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>7</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>7</v>
       </c>
@@ -1402,7 +1402,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>7</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>7</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>7</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>7</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>7</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>7</v>
       </c>
@@ -1483,7 +1483,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>7</v>
       </c>
@@ -1494,7 +1494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>8</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>8</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>8</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>8</v>
       </c>
@@ -1550,7 +1550,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>8</v>
       </c>
@@ -1559,7 +1559,7 @@
       </c>
       <c r="D76" s="3"/>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>8</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>8</v>
       </c>
@@ -1587,7 +1587,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>8</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="48.75" customHeight="1">
+    <row r="80" spans="1:10" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>8</v>
       </c>
@@ -1618,7 +1618,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>8</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>9</v>
       </c>
@@ -1643,7 +1643,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>9</v>
       </c>
@@ -1657,7 +1657,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>9</v>
       </c>
@@ -1671,7 +1671,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="84.75" customHeight="1">
+    <row r="85" spans="1:10" ht="84.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>9</v>
       </c>
@@ -1691,7 +1691,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>9</v>
       </c>
@@ -1702,7 +1702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>9</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>9</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>9</v>
       </c>
@@ -1744,7 +1744,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="105">
+    <row r="90" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>9</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>9</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="77.25" customHeight="1">
+    <row r="92" spans="1:10" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>10</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>10</v>
       </c>
@@ -1812,7 +1812,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>10</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>10</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>10</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="75.75" customHeight="1">
+    <row r="97" spans="1:10" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>10</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>10</v>
       </c>
@@ -1885,7 +1885,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>10</v>
       </c>
@@ -1899,7 +1899,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>10</v>
       </c>
@@ -1913,7 +1913,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>10</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>11</v>
       </c>
@@ -1938,7 +1938,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>11</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="104" spans="1:10">
+    <row r="104" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>11</v>
       </c>
@@ -1966,7 +1966,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="105" spans="1:10">
+    <row r="105" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>11</v>
       </c>
@@ -1980,7 +1980,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>11</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:10">
+    <row r="107" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>11</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>11</v>
       </c>
@@ -2019,7 +2019,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="109" spans="1:10">
+    <row r="109" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>11</v>
       </c>
@@ -2033,7 +2033,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="110" spans="1:10">
+    <row r="110" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>11</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>11</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="1:10">
+    <row r="112" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>12</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="113" spans="1:10">
+    <row r="113" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>12</v>
       </c>
@@ -2083,7 +2083,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="114" spans="1:10">
+    <row r="114" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>12</v>
       </c>
@@ -2097,7 +2097,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="115" spans="1:10">
+    <row r="115" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>12</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="116" spans="1:10">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>12</v>
       </c>
@@ -2122,7 +2122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:10">
+    <row r="117" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>12</v>
       </c>
@@ -2136,7 +2136,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="118" spans="1:10">
+    <row r="118" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>12</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="119" spans="1:10">
+    <row r="119" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>12</v>
       </c>
@@ -2164,7 +2164,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="120" spans="1:10">
+    <row r="120" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>12</v>
       </c>
@@ -2178,7 +2178,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="121" spans="1:10">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>12</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:10">
+    <row r="122" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>13</v>
       </c>
@@ -2203,7 +2203,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="123" spans="1:10">
+    <row r="123" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>13</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="124" spans="1:10">
+    <row r="124" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
         <v>13</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="125" spans="1:10">
+    <row r="125" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>13</v>
       </c>
@@ -2245,7 +2245,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="126" spans="1:10">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
         <v>13</v>
       </c>
@@ -2256,7 +2256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:10">
+    <row r="127" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
         <v>13</v>
       </c>
@@ -2270,7 +2270,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="128" spans="1:10">
+    <row r="128" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
         <v>13</v>
       </c>
@@ -2284,7 +2284,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="129" spans="1:10">
+    <row r="129" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>13</v>
       </c>
@@ -2298,7 +2298,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="130" spans="1:10">
+    <row r="130" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
         <v>13</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="131" spans="1:10">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
         <v>13</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:10">
+    <row r="132" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
         <v>14</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="133" spans="1:10">
+    <row r="133" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
         <v>14</v>
       </c>
@@ -2351,7 +2351,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="134" spans="1:10">
+    <row r="134" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
         <v>14</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="135" spans="1:10">
+    <row r="135" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
         <v>14</v>
       </c>
@@ -2379,7 +2379,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="136" spans="1:10">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
         <v>14</v>
       </c>
@@ -2390,7 +2390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:10">
+    <row r="137" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
         <v>14</v>
       </c>
@@ -2404,7 +2404,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="138" spans="1:10">
+    <row r="138" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
         <v>14</v>
       </c>
@@ -2418,7 +2418,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="139" spans="1:10">
+    <row r="139" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
         <v>14</v>
       </c>
@@ -2432,7 +2432,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="140" spans="1:10">
+    <row r="140" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
         <v>14</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="141" spans="1:10">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
         <v>14</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:10" ht="73.5" customHeight="1">
+    <row r="142" spans="1:10" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
         <v>15</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="143" spans="1:10">
+    <row r="143" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
         <v>15</v>
       </c>
@@ -2494,7 +2494,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="144" spans="1:10">
+    <row r="144" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
         <v>15</v>
       </c>
@@ -2508,7 +2508,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="145" spans="1:10">
+    <row r="145" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
         <v>15</v>
       </c>
@@ -2522,7 +2522,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="146" spans="1:10">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
         <v>15</v>
       </c>
@@ -2533,7 +2533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:10" ht="62.25" customHeight="1">
+    <row r="147" spans="1:10" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
         <v>15</v>
       </c>
@@ -2559,7 +2559,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="148" spans="1:10">
+    <row r="148" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
         <v>15</v>
       </c>
@@ -2573,7 +2573,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="149" spans="1:10">
+    <row r="149" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
         <v>15</v>
       </c>
@@ -2587,7 +2587,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="150" spans="1:10">
+    <row r="150" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
         <v>15</v>
       </c>
@@ -2601,7 +2601,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="151" spans="1:10">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
         <v>15</v>
       </c>
@@ -2612,7 +2612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:10">
+    <row r="152" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
         <v>16</v>
       </c>
@@ -2626,7 +2626,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="153" spans="1:10">
+    <row r="153" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
         <v>16</v>
       </c>
@@ -2640,7 +2640,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="154" spans="1:10">
+    <row r="154" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
         <v>16</v>
       </c>
@@ -2654,7 +2654,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="155" spans="1:10">
+    <row r="155" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
         <v>16</v>
       </c>
@@ -2668,7 +2668,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="156" spans="1:10">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
         <v>16</v>
       </c>
@@ -2679,7 +2679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:10">
+    <row r="157" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
         <v>16</v>
       </c>
@@ -2693,7 +2693,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="158" spans="1:10">
+    <row r="158" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
         <v>16</v>
       </c>
@@ -2707,7 +2707,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="159" spans="1:10">
+    <row r="159" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
         <v>16</v>
       </c>
@@ -2721,7 +2721,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="160" spans="1:10">
+    <row r="160" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
         <v>16</v>
       </c>
@@ -2735,7 +2735,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="161" spans="1:10">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
         <v>16</v>
       </c>
@@ -2746,7 +2746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:10" ht="72.75" customHeight="1">
+    <row r="162" spans="1:10" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
         <v>17</v>
       </c>
@@ -2763,7 +2763,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="163" spans="1:10">
+    <row r="163" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
         <v>17</v>
       </c>
@@ -2777,7 +2777,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="164" spans="1:10">
+    <row r="164" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
         <v>17</v>
       </c>
@@ -2791,7 +2791,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="165" spans="1:10">
+    <row r="165" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
         <v>17</v>
       </c>
@@ -2805,7 +2805,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="166" spans="1:10">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
         <v>17</v>
       </c>
@@ -2816,7 +2816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:10">
+    <row r="167" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
         <v>17</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="168" spans="1:10">
+    <row r="168" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
         <v>17</v>
       </c>
@@ -2844,7 +2844,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="169" spans="1:10">
+    <row r="169" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
         <v>17</v>
       </c>
@@ -2858,7 +2858,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="170" spans="1:10">
+    <row r="170" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
         <v>17</v>
       </c>
@@ -2872,7 +2872,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="171" spans="1:10">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
         <v>17</v>
       </c>
@@ -2883,7 +2883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:10">
+    <row r="172" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
         <v>18</v>
       </c>
@@ -2897,7 +2897,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="173" spans="1:10">
+    <row r="173" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
         <v>18</v>
       </c>
@@ -2911,7 +2911,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="174" spans="1:10">
+    <row r="174" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
         <v>18</v>
       </c>
@@ -2925,7 +2925,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="175" spans="1:10">
+    <row r="175" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
         <v>18</v>
       </c>
@@ -2939,7 +2939,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="176" spans="1:10">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
         <v>18</v>
       </c>
@@ -2950,7 +2950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:10">
+    <row r="177" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
         <v>18</v>
       </c>
@@ -2964,7 +2964,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="178" spans="1:10">
+    <row r="178" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
         <v>18</v>
       </c>
@@ -2978,7 +2978,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="179" spans="1:10">
+    <row r="179" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
         <v>18</v>
       </c>
@@ -2992,7 +2992,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="180" spans="1:10">
+    <row r="180" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
         <v>18</v>
       </c>
@@ -3006,7 +3006,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="181" spans="1:10">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
         <v>18</v>
       </c>
@@ -3014,7 +3014,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="182" spans="1:10">
+    <row r="182" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
         <v>19</v>
       </c>
@@ -3028,7 +3028,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="183" spans="1:10">
+    <row r="183" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
         <v>19</v>
       </c>
@@ -3042,7 +3042,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="184" spans="1:10">
+    <row r="184" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
         <v>19</v>
       </c>
@@ -3056,7 +3056,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="185" spans="1:10">
+    <row r="185" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
         <v>19</v>
       </c>
@@ -3070,7 +3070,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="186" spans="1:10">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
         <v>19</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:10">
+    <row r="187" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
         <v>19</v>
       </c>
@@ -3095,7 +3095,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="188" spans="1:10">
+    <row r="188" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
         <v>19</v>
       </c>
@@ -3109,7 +3109,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="189" spans="1:10">
+    <row r="189" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
         <v>19</v>
       </c>
@@ -3123,7 +3123,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="190" spans="1:10">
+    <row r="190" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
         <v>19</v>
       </c>
@@ -3137,7 +3137,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="191" spans="1:10">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
         <v>19</v>
       </c>
@@ -3148,7 +3148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:10">
+    <row r="192" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
         <v>20</v>
       </c>
@@ -3162,7 +3162,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="193" spans="1:10">
+    <row r="193" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
         <v>20</v>
       </c>
@@ -3176,7 +3176,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="194" spans="1:10">
+    <row r="194" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
         <v>20</v>
       </c>
@@ -3190,7 +3190,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="195" spans="1:10">
+    <row r="195" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
         <v>20</v>
       </c>
@@ -3204,7 +3204,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="196" spans="1:10">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
         <v>20</v>
       </c>
@@ -3212,7 +3212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:10">
+    <row r="197" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
         <v>20</v>
       </c>
@@ -3226,7 +3226,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="198" spans="1:10">
+    <row r="198" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
         <v>20</v>
       </c>
@@ -3240,7 +3240,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="199" spans="1:10">
+    <row r="199" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
         <v>20</v>
       </c>
@@ -3254,7 +3254,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="200" spans="1:10">
+    <row r="200" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
         <v>20</v>
       </c>
@@ -3268,7 +3268,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="201" spans="1:10">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
         <v>20</v>
       </c>
@@ -3276,7 +3276,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="202" spans="1:10" ht="75" customHeight="1">
+    <row r="202" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
         <v>21</v>
       </c>
@@ -3299,7 +3299,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="203" spans="1:10">
+    <row r="203" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
         <v>21</v>
       </c>
@@ -3313,7 +3313,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="204" spans="1:10">
+    <row r="204" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
         <v>21</v>
       </c>
@@ -3327,7 +3327,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="205" spans="1:10" ht="88.5" customHeight="1">
+    <row r="205" spans="1:10" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
         <v>21</v>
       </c>
@@ -3344,7 +3344,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="206" spans="1:10">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
         <v>21</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:10" ht="39" customHeight="1">
+    <row r="207" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
         <v>21</v>
       </c>
@@ -3372,7 +3372,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="208" spans="1:10">
+    <row r="208" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
         <v>21</v>
       </c>
@@ -3383,7 +3383,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="209" spans="1:10">
+    <row r="209" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A209" s="1">
         <v>21</v>
       </c>
@@ -3394,7 +3394,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="210" spans="1:10" ht="69" customHeight="1">
+    <row r="210" spans="1:10" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" s="1">
         <v>21</v>
       </c>
@@ -3414,7 +3414,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="211" spans="1:10">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
         <v>21</v>
       </c>
@@ -3425,7 +3425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:10">
+    <row r="212" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
         <v>22</v>
       </c>
@@ -3439,7 +3439,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="213" spans="1:10">
+    <row r="213" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
         <v>22</v>
       </c>
@@ -3453,7 +3453,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="214" spans="1:10">
+    <row r="214" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A214" s="1">
         <v>22</v>
       </c>
@@ -3467,7 +3467,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="215" spans="1:10">
+    <row r="215" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
         <v>22</v>
       </c>
@@ -3481,7 +3481,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="216" spans="1:10">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
         <v>22</v>
       </c>
@@ -3492,7 +3492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:10">
+    <row r="217" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
         <v>22</v>
       </c>
@@ -3506,7 +3506,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="218" spans="1:10">
+    <row r="218" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
         <v>22</v>
       </c>
@@ -3520,7 +3520,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="219" spans="1:10">
+    <row r="219" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A219" s="1">
         <v>22</v>
       </c>
@@ -3534,7 +3534,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="220" spans="1:10">
+    <row r="220" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
         <v>22</v>
       </c>
@@ -3548,7 +3548,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="221" spans="1:10">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
         <v>22</v>
       </c>
@@ -3556,7 +3556,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="222" spans="1:10">
+    <row r="222" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
         <v>23</v>
       </c>
@@ -3570,7 +3570,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="223" spans="1:10">
+    <row r="223" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A223" s="1">
         <v>23</v>
       </c>
@@ -3584,7 +3584,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="224" spans="1:10">
+    <row r="224" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A224" s="1">
         <v>23</v>
       </c>
@@ -3598,7 +3598,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="225" spans="1:10">
+    <row r="225" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A225" s="1">
         <v>23</v>
       </c>
@@ -3612,7 +3612,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="226" spans="1:10">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A226" s="1">
         <v>23</v>
       </c>
@@ -3623,7 +3623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:10">
+    <row r="227" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A227" s="1">
         <v>23</v>
       </c>
@@ -3637,7 +3637,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="228" spans="1:10">
+    <row r="228" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A228" s="1">
         <v>23</v>
       </c>
@@ -3651,7 +3651,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="229" spans="1:10">
+    <row r="229" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A229" s="1">
         <v>23</v>
       </c>
@@ -3665,7 +3665,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="230" spans="1:10">
+    <row r="230" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A230" s="1">
         <v>23</v>
       </c>
@@ -3679,7 +3679,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="231" spans="1:10">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A231" s="1">
         <v>23</v>
       </c>
@@ -3690,7 +3690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:10" ht="77.25" customHeight="1">
+    <row r="232" spans="1:10" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A232" s="1">
         <v>24</v>
       </c>
@@ -3707,7 +3707,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="233" spans="1:10">
+    <row r="233" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A233" s="1">
         <v>24</v>
       </c>
@@ -3721,7 +3721,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="234" spans="1:10">
+    <row r="234" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A234" s="1">
         <v>24</v>
       </c>
@@ -3735,7 +3735,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="235" spans="1:10">
+    <row r="235" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A235" s="1">
         <v>24</v>
       </c>
@@ -3749,7 +3749,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="236" spans="1:10">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A236" s="1">
         <v>24</v>
       </c>
@@ -3757,7 +3757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:10">
+    <row r="237" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A237" s="1">
         <v>24</v>
       </c>
@@ -3771,7 +3771,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="238" spans="1:10">
+    <row r="238" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A238" s="1">
         <v>24</v>
       </c>
@@ -3785,7 +3785,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="239" spans="1:10">
+    <row r="239" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A239" s="1">
         <v>24</v>
       </c>
@@ -3799,7 +3799,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="240" spans="1:10">
+    <row r="240" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A240" s="1">
         <v>24</v>
       </c>
@@ -3813,7 +3813,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="241" spans="1:10">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A241" s="1">
         <v>24</v>
       </c>
@@ -3821,7 +3821,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="242" spans="1:10">
+    <row r="242" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A242" s="1">
         <v>25</v>
       </c>
@@ -3835,7 +3835,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="243" spans="1:10">
+    <row r="243" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A243" s="1">
         <v>25</v>
       </c>
@@ -3849,7 +3849,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="244" spans="1:10">
+    <row r="244" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A244" s="1">
         <v>25</v>
       </c>
@@ -3863,7 +3863,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="245" spans="1:10">
+    <row r="245" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A245" s="1">
         <v>25</v>
       </c>
@@ -3877,7 +3877,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="246" spans="1:10">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A246" s="1">
         <v>25</v>
       </c>
@@ -3888,7 +3888,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="247" spans="1:10">
+    <row r="247" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A247" s="1">
         <v>25</v>
       </c>
@@ -3902,7 +3902,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="248" spans="1:10">
+    <row r="248" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A248" s="1">
         <v>25</v>
       </c>
@@ -3916,7 +3916,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="249" spans="1:10">
+    <row r="249" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A249" s="1">
         <v>25</v>
       </c>
@@ -3930,7 +3930,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="250" spans="1:10">
+    <row r="250" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A250" s="1">
         <v>25</v>
       </c>
@@ -3944,7 +3944,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="251" spans="1:10">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A251" s="1">
         <v>25</v>
       </c>
@@ -3955,7 +3955,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="252" spans="1:10" ht="29.25" customHeight="1">
+    <row r="252" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A252" s="1">
         <v>26</v>
       </c>
@@ -3972,7 +3972,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="253" spans="1:10">
+    <row r="253" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A253" s="1">
         <v>26</v>
       </c>
@@ -3986,7 +3986,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="254" spans="1:10">
+    <row r="254" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A254" s="1">
         <v>26</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="255" spans="1:10">
+    <row r="255" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A255" s="1">
         <v>26</v>
       </c>
@@ -4014,7 +4014,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="256" spans="1:10">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A256" s="1">
         <v>26</v>
       </c>
@@ -4025,7 +4025,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="257" spans="1:10" ht="43.5" customHeight="1">
+    <row r="257" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A257" s="1">
         <v>26</v>
       </c>
@@ -4042,7 +4042,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="258" spans="1:10">
+    <row r="258" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A258" s="1">
         <v>26</v>
       </c>
@@ -4056,7 +4056,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="259" spans="1:10">
+    <row r="259" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A259" s="1">
         <v>26</v>
       </c>
@@ -4070,7 +4070,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="260" spans="1:10">
+    <row r="260" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A260" s="1">
         <v>26</v>
       </c>
@@ -4084,7 +4084,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="261" spans="1:10">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A261" s="1">
         <v>26</v>
       </c>
@@ -4095,7 +4095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:10" ht="72.75" customHeight="1">
+    <row r="262" spans="1:10" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A262" s="1">
         <v>27</v>
       </c>
@@ -4115,7 +4115,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="263" spans="1:10">
+    <row r="263" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A263" s="1">
         <v>27</v>
       </c>
@@ -4129,7 +4129,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="264" spans="1:10">
+    <row r="264" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A264" s="1">
         <v>27</v>
       </c>
@@ -4143,7 +4143,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="265" spans="1:10">
+    <row r="265" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A265" s="1">
         <v>27</v>
       </c>
@@ -4157,7 +4157,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="266" spans="1:10">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A266" s="1">
         <v>27</v>
       </c>
@@ -4165,7 +4165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:10" ht="74.25" customHeight="1">
+    <row r="267" spans="1:10" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A267" s="1">
         <v>27</v>
       </c>
@@ -4185,7 +4185,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="268" spans="1:10">
+    <row r="268" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A268" s="1">
         <v>27</v>
       </c>
@@ -4199,7 +4199,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="269" spans="1:10">
+    <row r="269" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A269" s="1">
         <v>27</v>
       </c>
@@ -4213,7 +4213,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="270" spans="1:10">
+    <row r="270" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A270" s="1">
         <v>27</v>
       </c>
@@ -4227,7 +4227,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="271" spans="1:10">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A271" s="1">
         <v>27</v>
       </c>
@@ -4238,7 +4238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:10" ht="72.75" customHeight="1">
+    <row r="272" spans="1:10" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A272" s="1">
         <v>28</v>
       </c>
@@ -4258,7 +4258,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="273" spans="1:10">
+    <row r="273" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A273" s="1">
         <v>28</v>
       </c>
@@ -4272,7 +4272,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="274" spans="1:10">
+    <row r="274" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A274" s="1">
         <v>28</v>
       </c>
@@ -4286,7 +4286,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="275" spans="1:10">
+    <row r="275" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A275" s="1">
         <v>28</v>
       </c>
@@ -4300,7 +4300,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="276" spans="1:10">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A276" s="1">
         <v>28</v>
       </c>
@@ -4308,7 +4308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:10" ht="72" customHeight="1">
+    <row r="277" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A277" s="1">
         <v>28</v>
       </c>
@@ -4328,7 +4328,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="278" spans="1:10">
+    <row r="278" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A278" s="1">
         <v>28</v>
       </c>
@@ -4342,7 +4342,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="279" spans="1:10">
+    <row r="279" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A279" s="1">
         <v>28</v>
       </c>
@@ -4356,7 +4356,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="280" spans="1:10">
+    <row r="280" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A280" s="1">
         <v>28</v>
       </c>
@@ -4370,7 +4370,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="281" spans="1:10">
+    <row r="281" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A281" s="1">
         <v>28</v>
       </c>
@@ -4378,7 +4378,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="282" spans="1:10">
+    <row r="282" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A282" s="1">
         <v>29</v>
       </c>
@@ -4392,7 +4392,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="283" spans="1:10">
+    <row r="283" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A283" s="1">
         <v>29</v>
       </c>
@@ -4406,7 +4406,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="284" spans="1:10">
+    <row r="284" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A284" s="1">
         <v>29</v>
       </c>
@@ -4420,7 +4420,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="285" spans="1:10">
+    <row r="285" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A285" s="1">
         <v>29</v>
       </c>
@@ -4434,7 +4434,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="286" spans="1:10">
+    <row r="286" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A286" s="1">
         <v>29</v>
       </c>
@@ -4445,7 +4445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:10">
+    <row r="287" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A287" s="1">
         <v>29</v>
       </c>
@@ -4459,7 +4459,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="288" spans="1:10">
+    <row r="288" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A288" s="1">
         <v>29</v>
       </c>
@@ -4473,7 +4473,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="289" spans="1:10">
+    <row r="289" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A289" s="1">
         <v>29</v>
       </c>
@@ -4487,7 +4487,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="290" spans="1:10">
+    <row r="290" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A290" s="1">
         <v>29</v>
       </c>
@@ -4501,7 +4501,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="291" spans="1:10">
+    <row r="291" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A291" s="1">
         <v>29</v>
       </c>
@@ -4512,7 +4512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="1:10">
+    <row r="292" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A292" s="1">
         <v>30</v>
       </c>
@@ -4526,7 +4526,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="293" spans="1:10">
+    <row r="293" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A293" s="1">
         <v>30</v>
       </c>
@@ -4540,7 +4540,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="294" spans="1:10">
+    <row r="294" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A294" s="1">
         <v>30</v>
       </c>
@@ -4554,7 +4554,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="295" spans="1:10">
+    <row r="295" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A295" s="1">
         <v>30</v>
       </c>
@@ -4568,7 +4568,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="296" spans="1:10">
+    <row r="296" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A296" s="1">
         <v>30</v>
       </c>
@@ -4579,7 +4579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:10" ht="69.75" customHeight="1">
+    <row r="297" spans="1:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A297" s="1">
         <v>30</v>
       </c>
@@ -4596,7 +4596,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="298" spans="1:10">
+    <row r="298" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A298" s="1">
         <v>30</v>
       </c>
@@ -4610,7 +4610,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="299" spans="1:10">
+    <row r="299" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A299" s="1">
         <v>30</v>
       </c>
@@ -4624,7 +4624,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="300" spans="1:10">
+    <row r="300" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A300" s="1">
         <v>30</v>
       </c>
@@ -4638,7 +4638,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="301" spans="1:10">
+    <row r="301" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A301" s="1">
         <v>30</v>
       </c>
@@ -4649,7 +4649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="302" spans="1:10">
+    <row r="302" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A302" s="1">
         <v>31</v>
       </c>
@@ -4663,7 +4663,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="303" spans="1:10">
+    <row r="303" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A303" s="1">
         <v>31</v>
       </c>
@@ -4677,7 +4677,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="304" spans="1:10">
+    <row r="304" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A304" s="1">
         <v>31</v>
       </c>
@@ -4691,7 +4691,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="305" spans="1:10">
+    <row r="305" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A305" s="1">
         <v>31</v>
       </c>
@@ -4705,7 +4705,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="306" spans="1:10">
+    <row r="306" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A306" s="1">
         <v>31</v>
       </c>
@@ -4716,7 +4716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:10" ht="77.25" customHeight="1">
+    <row r="307" spans="1:10" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A307" s="1">
         <v>31</v>
       </c>
@@ -4733,7 +4733,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="308" spans="1:10">
+    <row r="308" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A308" s="1">
         <v>31</v>
       </c>
@@ -4743,8 +4743,11 @@
       <c r="C308" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="309" spans="1:10">
+      <c r="D308" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="309" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A309" s="1">
         <v>31</v>
       </c>
@@ -4754,8 +4757,11 @@
       <c r="C309" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="310" spans="1:10">
+      <c r="D309" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="310" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A310" s="1">
         <v>31</v>
       </c>
@@ -4765,8 +4771,11 @@
       <c r="C310" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="311" spans="1:10">
+      <c r="D310" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="311" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A311" s="1">
         <v>31</v>
       </c>
@@ -4777,7 +4786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:10" ht="33.75" customHeight="1">
+    <row r="312" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A312" s="1">
         <v>32</v>
       </c>
@@ -4794,7 +4803,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="313" spans="1:10">
+    <row r="313" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A313" s="1">
         <v>32</v>
       </c>
@@ -4808,7 +4817,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="314" spans="1:10">
+    <row r="314" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A314" s="1">
         <v>32</v>
       </c>
@@ -4822,7 +4831,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="315" spans="1:10" ht="43.5" customHeight="1">
+    <row r="315" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A315" s="1">
         <v>32</v>
       </c>
@@ -4839,7 +4848,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="316" spans="1:10">
+    <row r="316" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A316" s="1">
         <v>32</v>
       </c>
@@ -4847,7 +4856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="317" spans="1:10">
+    <row r="317" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A317" s="1">
         <v>32</v>
       </c>
@@ -4861,7 +4870,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="318" spans="1:10">
+    <row r="318" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A318" s="1">
         <v>32</v>
       </c>
@@ -4875,7 +4884,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="319" spans="1:10">
+    <row r="319" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A319" s="1">
         <v>32</v>
       </c>
@@ -4889,7 +4898,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="320" spans="1:10" ht="44.25" customHeight="1">
+    <row r="320" spans="1:10" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A320" s="1">
         <v>32</v>
       </c>
@@ -4906,7 +4915,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="321" spans="1:10">
+    <row r="321" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A321" s="1">
         <v>32</v>
       </c>
@@ -4917,7 +4926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="322" spans="1:10" ht="71.25" customHeight="1">
+    <row r="322" spans="1:10" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A322" s="1">
         <v>33</v>
       </c>
@@ -4934,7 +4943,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="323" spans="1:10">
+    <row r="323" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A323" s="1">
         <v>33</v>
       </c>
@@ -4948,7 +4957,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="324" spans="1:10">
+    <row r="324" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A324" s="1">
         <v>33</v>
       </c>
@@ -4962,7 +4971,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="325" spans="1:10">
+    <row r="325" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A325" s="1">
         <v>33</v>
       </c>
@@ -4976,7 +4985,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="326" spans="1:10">
+    <row r="326" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A326" s="1">
         <v>33</v>
       </c>
@@ -4984,7 +4993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="327" spans="1:10" ht="69" customHeight="1">
+    <row r="327" spans="1:10" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A327" s="1">
         <v>33</v>
       </c>
@@ -4995,30 +5004,30 @@
         <v>10</v>
       </c>
       <c r="D327" s="1" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="F327" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H327" s="1" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="I327" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="328" spans="1:10" ht="48.75" customHeight="1">
+    <row r="328" spans="1:10" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D328" s="1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F328" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="H328" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="I328" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="329" spans="1:10">
+    <row r="329" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A329" s="1">
         <v>33</v>
       </c>
@@ -5032,7 +5041,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="330" spans="1:10">
+    <row r="330" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A330" s="1">
         <v>33</v>
       </c>
@@ -5046,7 +5055,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="331" spans="1:10">
+    <row r="331" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A331" s="1">
         <v>33</v>
       </c>
@@ -5060,7 +5069,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="332" spans="1:10">
+    <row r="332" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A332" s="1">
         <v>33</v>
       </c>
@@ -5071,7 +5080,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="333" spans="1:10" ht="27.75" customHeight="1">
+    <row r="333" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A333" s="1">
         <v>34</v>
       </c>
@@ -5088,7 +5097,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="334" spans="1:10">
+    <row r="334" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A334" s="1">
         <v>34</v>
       </c>
@@ -5102,7 +5111,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="335" spans="1:10">
+    <row r="335" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A335" s="1">
         <v>34</v>
       </c>
@@ -5116,7 +5125,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="336" spans="1:10">
+    <row r="336" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A336" s="1">
         <v>34</v>
       </c>
@@ -5130,7 +5139,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="337" spans="1:10">
+    <row r="337" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A337" s="1">
         <v>34</v>
       </c>
@@ -5141,7 +5150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="338" spans="1:10" ht="36" customHeight="1">
+    <row r="338" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A338" s="1">
         <v>34</v>
       </c>
@@ -5158,7 +5167,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="339" spans="1:10">
+    <row r="339" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A339" s="1">
         <v>34</v>
       </c>
@@ -5172,7 +5181,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="340" spans="1:10">
+    <row r="340" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A340" s="1">
         <v>34</v>
       </c>
@@ -5186,7 +5195,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="341" spans="1:10">
+    <row r="341" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A341" s="1">
         <v>34</v>
       </c>
@@ -5200,7 +5209,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="342" spans="1:10">
+    <row r="342" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A342" s="1">
         <v>34</v>
       </c>
@@ -5211,7 +5220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="343" spans="1:10">
+    <row r="343" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A343" s="1">
         <v>35</v>
       </c>
@@ -5225,7 +5234,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="344" spans="1:10">
+    <row r="344" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A344" s="1">
         <v>35</v>
       </c>
@@ -5239,7 +5248,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="345" spans="1:10">
+    <row r="345" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A345" s="1">
         <v>35</v>
       </c>
@@ -5253,7 +5262,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="346" spans="1:10">
+    <row r="346" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A346" s="1">
         <v>35</v>
       </c>
@@ -5267,7 +5276,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="347" spans="1:10">
+    <row r="347" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A347" s="1">
         <v>35</v>
       </c>
@@ -5278,7 +5287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="348" spans="1:10">
+    <row r="348" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A348" s="1">
         <v>35</v>
       </c>
@@ -5292,7 +5301,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="349" spans="1:10">
+    <row r="349" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A349" s="1">
         <v>35</v>
       </c>
@@ -5306,7 +5315,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="350" spans="1:10">
+    <row r="350" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A350" s="1">
         <v>35</v>
       </c>
@@ -5320,7 +5329,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="351" spans="1:10">
+    <row r="351" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A351" s="1">
         <v>35</v>
       </c>
@@ -5334,7 +5343,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="352" spans="1:10">
+    <row r="352" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A352" s="1">
         <v>35</v>
       </c>
@@ -5345,7 +5354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="353" spans="1:10" ht="86.25" customHeight="1">
+    <row r="353" spans="1:10" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A353" s="1">
         <v>36</v>
       </c>
@@ -5362,7 +5371,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="354" spans="1:10">
+    <row r="354" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A354" s="1">
         <v>36</v>
       </c>
@@ -5376,7 +5385,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="355" spans="1:10">
+    <row r="355" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A355" s="1">
         <v>36</v>
       </c>
@@ -5390,7 +5399,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="356" spans="1:10">
+    <row r="356" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A356" s="1">
         <v>36</v>
       </c>
@@ -5404,7 +5413,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="357" spans="1:10">
+    <row r="357" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A357" s="1">
         <v>36</v>
       </c>
@@ -5415,7 +5424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="358" spans="1:10" ht="79.5" customHeight="1">
+    <row r="358" spans="1:10" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A358" s="1">
         <v>36</v>
       </c>
@@ -5432,7 +5441,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="359" spans="1:10">
+    <row r="359" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A359" s="1">
         <v>36</v>
       </c>
@@ -5446,7 +5455,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="360" spans="1:10">
+    <row r="360" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A360" s="1">
         <v>36</v>
       </c>
@@ -5460,7 +5469,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="361" spans="1:10">
+    <row r="361" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A361" s="1">
         <v>36</v>
       </c>
@@ -5477,7 +5486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="362" spans="1:10">
+    <row r="362" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A362" s="1">
         <v>36</v>
       </c>
@@ -5485,7 +5494,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="363" spans="1:10" ht="82.5" customHeight="1">
+    <row r="363" spans="1:10" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A363" s="1">
         <v>37</v>
       </c>
@@ -5505,7 +5514,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="364" spans="1:10">
+    <row r="364" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A364" s="1">
         <v>37</v>
       </c>
@@ -5519,7 +5528,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="365" spans="1:10">
+    <row r="365" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A365" s="1">
         <v>37</v>
       </c>
@@ -5533,7 +5542,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="366" spans="1:10">
+    <row r="366" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A366" s="1">
         <v>37</v>
       </c>
@@ -5547,7 +5556,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="367" spans="1:10">
+    <row r="367" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A367" s="1">
         <v>37</v>
       </c>
@@ -5558,7 +5567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="368" spans="1:10">
+    <row r="368" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A368" s="1">
         <v>37</v>
       </c>
@@ -5572,7 +5581,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="369" spans="1:10">
+    <row r="369" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A369" s="1">
         <v>37</v>
       </c>
@@ -5586,7 +5595,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="370" spans="1:10">
+    <row r="370" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A370" s="1">
         <v>37</v>
       </c>
@@ -5600,7 +5609,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="371" spans="1:10">
+    <row r="371" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A371" s="1">
         <v>37</v>
       </c>
@@ -5614,7 +5623,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="372" spans="1:10">
+    <row r="372" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A372" s="1">
         <v>37</v>
       </c>
@@ -5622,7 +5631,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="373" spans="1:10" ht="81" customHeight="1">
+    <row r="373" spans="1:10" ht="81" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A373" s="1">
         <v>38</v>
       </c>
@@ -5642,7 +5651,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="374" spans="1:10">
+    <row r="374" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A374" s="1">
         <v>38</v>
       </c>
@@ -5656,7 +5665,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="375" spans="1:10">
+    <row r="375" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A375" s="1">
         <v>38</v>
       </c>
@@ -5670,7 +5679,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="376" spans="1:10">
+    <row r="376" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A376" s="1">
         <v>38</v>
       </c>
@@ -5684,7 +5693,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="377" spans="1:10">
+    <row r="377" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A377" s="1">
         <v>38</v>
       </c>
@@ -5695,7 +5704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="378" spans="1:10" ht="28.5" customHeight="1">
+    <row r="378" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A378" s="1">
         <v>38</v>
       </c>
@@ -5712,7 +5721,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="379" spans="1:10">
+    <row r="379" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A379" s="1">
         <v>38</v>
       </c>
@@ -5726,7 +5735,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="380" spans="1:10">
+    <row r="380" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A380" s="1">
         <v>38</v>
       </c>
@@ -5740,7 +5749,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="381" spans="1:10">
+    <row r="381" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A381" s="1">
         <v>38</v>
       </c>
@@ -5754,7 +5763,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="382" spans="1:10">
+    <row r="382" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A382" s="1">
         <v>38</v>
       </c>
@@ -5765,7 +5774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="383" spans="1:10">
+    <row r="383" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A383" s="1">
         <v>39</v>
       </c>
@@ -5779,7 +5788,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="384" spans="1:10">
+    <row r="384" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A384" s="1">
         <v>39</v>
       </c>
@@ -5793,7 +5802,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="385" spans="1:10">
+    <row r="385" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A385" s="1">
         <v>39</v>
       </c>
@@ -5807,7 +5816,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="386" spans="1:10">
+    <row r="386" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A386" s="1">
         <v>39</v>
       </c>
@@ -5821,7 +5830,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="387" spans="1:10">
+    <row r="387" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A387" s="1">
         <v>39</v>
       </c>
@@ -5829,7 +5838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="388" spans="1:10">
+    <row r="388" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A388" s="1">
         <v>39</v>
       </c>
@@ -5843,7 +5852,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="389" spans="1:10">
+    <row r="389" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A389" s="1">
         <v>39</v>
       </c>
@@ -5857,7 +5866,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="390" spans="1:10">
+    <row r="390" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A390" s="1">
         <v>39</v>
       </c>
@@ -5871,7 +5880,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="391" spans="1:10">
+    <row r="391" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A391" s="1">
         <v>39</v>
       </c>
@@ -5885,7 +5894,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="392" spans="1:10">
+    <row r="392" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A392" s="1">
         <v>39</v>
       </c>
@@ -5896,7 +5905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="393" spans="1:10">
+    <row r="393" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A393" s="1">
         <v>40</v>
       </c>
@@ -5910,7 +5919,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="394" spans="1:10">
+    <row r="394" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A394" s="1">
         <v>40</v>
       </c>
@@ -5924,7 +5933,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="395" spans="1:10">
+    <row r="395" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A395" s="1">
         <v>40</v>
       </c>
@@ -5938,7 +5947,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="396" spans="1:10">
+    <row r="396" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A396" s="1">
         <v>40</v>
       </c>
@@ -5952,7 +5961,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="397" spans="1:10">
+    <row r="397" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A397" s="1">
         <v>40</v>
       </c>
@@ -5960,7 +5969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="398" spans="1:10">
+    <row r="398" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A398" s="1">
         <v>40</v>
       </c>
@@ -5974,7 +5983,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="399" spans="1:10">
+    <row r="399" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A399" s="1">
         <v>40</v>
       </c>
@@ -5988,7 +5997,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="400" spans="1:10">
+    <row r="400" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A400" s="1">
         <v>40</v>
       </c>
@@ -6002,7 +6011,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="401" spans="1:4">
+    <row r="401" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A401" s="1">
         <v>40</v>
       </c>
@@ -6016,7 +6025,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="402" spans="1:4">
+    <row r="402" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A402" s="1">
         <v>40</v>
       </c>

</xml_diff>